<commit_message>
Parameters Setting - Hybrid
</commit_message>
<xml_diff>
--- a/Parameters Setting/Parameters Setting.xlsx
+++ b/Parameters Setting/Parameters Setting.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inosoft_04\Desktop\Parameters Setting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inosoft_04\Desktop\PAPER\MATLAB\Parameters Setting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FF8F8A-1EB0-4CDF-BAF1-FBCE584EE82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD9F30C-8DC4-44A5-ABD0-F6FEC0C41C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EC36AE17-BCB7-4062-8E47-F0BBC63F2042}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC36AE17-BCB7-4062-8E47-F0BBC63F2042}"/>
   </bookViews>
   <sheets>
     <sheet name="NSGA-II" sheetId="1" r:id="rId1"/>
+    <sheet name="Hybrid" sheetId="2" r:id="rId2"/>
+    <sheet name="MOEA-D" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>SNS</t>
   </si>
@@ -70,6 +72,24 @@
   </si>
   <si>
     <t>Row</t>
+  </si>
+  <si>
+    <t>Max_subit</t>
+  </si>
+  <si>
+    <t>T_0</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>TL_size</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -255,12 +275,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -287,9 +307,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -321,6 +338,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -640,7 +690,7 @@
   <dimension ref="B3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,42 +711,64 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="4" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="20" t="s">
         <v>6</v>
       </c>
     </row>
@@ -719,22 +791,24 @@
       <c r="G5" s="10">
         <v>12.4168</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="1">
         <v>25</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="1">
         <v>0.83003000000000005</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="1">
         <v>223.31010000000001</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="1">
         <v>0.29076999999999997</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="1">
         <v>0.14061000000000001</v>
       </c>
-      <c r="M5" s="12"/>
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
@@ -755,22 +829,24 @@
       <c r="G6" s="10">
         <v>24.863399999999999</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="1">
         <v>39</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="1">
         <v>0.52261999999999997</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="1">
         <v>590.58339999999998</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="1">
         <v>0.22109999999999999</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="1">
         <v>0.25197999999999998</v>
       </c>
-      <c r="M6" s="12"/>
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -791,22 +867,24 @@
       <c r="G7" s="10">
         <v>46.671399999999998</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="1">
         <v>34</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="1">
         <v>0.63549999999999995</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="1">
         <v>406.33949999999999</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="1">
         <v>0.25392999999999999</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="1">
         <v>0.20347000000000001</v>
       </c>
-      <c r="M7" s="12"/>
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
@@ -827,22 +905,24 @@
       <c r="G8" s="10">
         <v>69.066800000000001</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="1">
         <v>29</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="1">
         <v>0.64956999999999998</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="1">
         <v>341.83870000000002</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="1">
         <v>0.2782</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="1">
         <v>0.17818999999999999</v>
       </c>
-      <c r="M8" s="12"/>
+      <c r="M8" s="11">
+        <v>0.2069</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
@@ -863,22 +943,24 @@
       <c r="G9" s="10">
         <v>31.617899999999999</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="1">
         <v>12</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="1">
         <v>0.84238000000000002</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="1">
         <v>94.519800000000004</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="1">
         <v>0.30092000000000002</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="1">
         <v>5.6675999999999997E-2</v>
       </c>
-      <c r="M9" s="12"/>
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
@@ -899,22 +981,24 @@
       <c r="G10" s="10">
         <v>51.110999999999997</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="1">
         <v>17</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="1">
         <v>0.86946999999999997</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="1">
         <v>138.34639999999999</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="1">
         <v>0.21809999999999999</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="1">
         <v>0.10258</v>
       </c>
-      <c r="M10" s="12"/>
+      <c r="M10" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
@@ -935,22 +1019,24 @@
       <c r="G11" s="10">
         <v>86.098500000000001</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="1">
         <v>17</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="1">
         <v>0.69111</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="1">
         <v>158.11060000000001</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="1">
         <v>0.24859999999999999</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="1">
         <v>7.8467999999999996E-2</v>
       </c>
-      <c r="M11" s="12"/>
+      <c r="M11" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
@@ -971,22 +1057,24 @@
       <c r="G12" s="10">
         <v>112.96080000000001</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="1">
         <v>25</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="1">
         <v>0.92949000000000004</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="1">
         <v>142.74080000000001</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="1">
         <v>0.19689000000000001</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="1">
         <v>0.10976</v>
       </c>
-      <c r="M12" s="12"/>
+      <c r="M12" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
@@ -1007,22 +1095,24 @@
       <c r="G13" s="10">
         <v>28.2</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="1">
         <v>19</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="1">
         <v>0.57755000000000001</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="1">
         <v>281.95400000000001</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="1">
         <v>0.31096000000000001</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="1">
         <v>0.12665999999999999</v>
       </c>
-      <c r="M13" s="12"/>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -1043,22 +1133,24 @@
       <c r="G14" s="10">
         <v>48.784199999999998</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="1">
         <v>26</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="1">
         <v>0.62587999999999999</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="1">
         <v>326.5521</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="1">
         <v>0.23916999999999999</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="1">
         <v>0.16894000000000001</v>
       </c>
-      <c r="M14" s="12"/>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -1079,22 +1171,24 @@
       <c r="G15" s="10">
         <v>56.974499999999999</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="1">
         <v>35</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="1">
         <v>0.66364000000000001</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="1">
         <v>224.87289999999999</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="1">
         <v>0.15617</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="1">
         <v>0.13231000000000001</v>
       </c>
-      <c r="M15" s="12"/>
+      <c r="M15" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
@@ -1115,22 +1209,24 @@
       <c r="G16" s="10">
         <v>74.706999999999994</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="1">
         <v>37</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="1">
         <v>0.59711999999999998</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="1">
         <v>367.2878</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="1">
         <v>0.35198000000000002</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="1">
         <v>0.1759</v>
       </c>
-      <c r="M16" s="12"/>
+      <c r="M16" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
@@ -1151,22 +1247,24 @@
       <c r="G17" s="10">
         <v>40.712000000000003</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="1">
         <v>26</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="1">
         <v>0.69386999999999999</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="1">
         <v>281.56979999999999</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="1">
         <v>0.32466</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="1">
         <v>0.16875999999999999</v>
       </c>
-      <c r="M17" s="12"/>
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
@@ -1187,22 +1285,24 @@
       <c r="G18" s="10">
         <v>56.531100000000002</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="1">
         <v>41</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="1">
         <v>0.68442999999999998</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="1">
         <v>336.93029999999999</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="1">
         <v>0.16666</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="1">
         <v>0.20494000000000001</v>
       </c>
-      <c r="M18" s="12"/>
+      <c r="M18" s="11">
+        <v>9.7600000000000006E-2</v>
+      </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
@@ -1223,22 +1323,24 @@
       <c r="G19" s="10">
         <v>112.79</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="1">
         <v>38</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="1">
         <v>0.56925999999999999</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="1">
         <v>264.3254</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="1">
         <v>0.22305</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="1">
         <v>0.12139</v>
       </c>
-      <c r="M19" s="12"/>
+      <c r="M19" s="11">
+        <v>2.63E-2</v>
+      </c>
     </row>
     <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
@@ -1256,29 +1358,1128 @@
       <c r="F20" s="9">
         <v>0.4</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="12">
         <v>121.50409999999999</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <v>28</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <v>0.51934000000000002</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <v>311.80360000000002</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="13">
         <v>0.24510999999999999</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="13">
         <v>0.11491999999999999</v>
       </c>
-      <c r="M20" s="15"/>
+      <c r="M20" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A78958-75F4-4D61-9D38-2A143FDEA36C}">
+  <dimension ref="B3:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="H3:N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <v>50</v>
+      </c>
+      <c r="D5" s="22">
+        <v>15</v>
+      </c>
+      <c r="E5" s="22">
+        <v>110</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0.87</v>
+      </c>
+      <c r="G5" s="23">
+        <v>3</v>
+      </c>
+      <c r="H5" s="24">
+        <v>17.463200000000001</v>
+      </c>
+      <c r="I5" s="1">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.0535000000000001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>147.29179999999999</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.23268</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.10600999999999999</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22">
+        <v>50</v>
+      </c>
+      <c r="D6" s="22">
+        <v>20</v>
+      </c>
+      <c r="E6" s="22">
+        <v>130</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="23">
+        <v>4</v>
+      </c>
+      <c r="H6" s="24">
+        <v>18.5412</v>
+      </c>
+      <c r="I6" s="1">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.56855999999999995</v>
+      </c>
+      <c r="K6" s="1">
+        <v>170.48699999999999</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.37468000000000001</v>
+      </c>
+      <c r="M6" s="1">
+        <v>7.1951000000000001E-2</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="22">
+        <v>50</v>
+      </c>
+      <c r="D7" s="22">
+        <v>25</v>
+      </c>
+      <c r="E7" s="22">
+        <v>150</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.93</v>
+      </c>
+      <c r="G7" s="23">
+        <v>5</v>
+      </c>
+      <c r="H7" s="24">
+        <v>20.0779</v>
+      </c>
+      <c r="I7" s="1">
+        <v>15</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.1894</v>
+      </c>
+      <c r="K7" s="1">
+        <v>98.278099999999995</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.14802999999999999</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.1231</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="22">
+        <v>50</v>
+      </c>
+      <c r="D8" s="22">
+        <v>30</v>
+      </c>
+      <c r="E8" s="22">
+        <v>170</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.96</v>
+      </c>
+      <c r="G8" s="23">
+        <v>6</v>
+      </c>
+      <c r="H8" s="24">
+        <v>25.283000000000001</v>
+      </c>
+      <c r="I8" s="1">
+        <v>15</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.84289999999999998</v>
+      </c>
+      <c r="K8" s="1">
+        <v>189.7508</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.26395999999999997</v>
+      </c>
+      <c r="M8" s="1">
+        <v>6.7584000000000005E-2</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="22">
+        <v>80</v>
+      </c>
+      <c r="D9" s="22">
+        <v>15</v>
+      </c>
+      <c r="E9" s="22">
+        <v>130</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.93</v>
+      </c>
+      <c r="G9" s="23">
+        <v>6</v>
+      </c>
+      <c r="H9" s="24">
+        <v>20.0792</v>
+      </c>
+      <c r="I9" s="1">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.0286</v>
+      </c>
+      <c r="K9" s="1">
+        <v>209.7544</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.23549999999999999</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.13141</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="22">
+        <v>80</v>
+      </c>
+      <c r="D10" s="22">
+        <v>20</v>
+      </c>
+      <c r="E10" s="22">
+        <v>110</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0.96</v>
+      </c>
+      <c r="G10" s="23">
+        <v>5</v>
+      </c>
+      <c r="H10" s="24">
+        <v>25.461200000000002</v>
+      </c>
+      <c r="I10" s="1">
+        <v>27</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.92554000000000003</v>
+      </c>
+      <c r="K10" s="1">
+        <v>314.47680000000003</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.17737</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="22">
+        <v>80</v>
+      </c>
+      <c r="D11" s="22">
+        <v>25</v>
+      </c>
+      <c r="E11" s="22">
+        <v>170</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0.87</v>
+      </c>
+      <c r="G11" s="23">
+        <v>4</v>
+      </c>
+      <c r="H11" s="24">
+        <v>30.334800000000001</v>
+      </c>
+      <c r="I11" s="1">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.0662</v>
+      </c>
+      <c r="K11" s="1">
+        <v>305.14980000000003</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.12806000000000001</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.18451000000000001</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12" s="22">
+        <v>80</v>
+      </c>
+      <c r="D12" s="22">
+        <v>30</v>
+      </c>
+      <c r="E12" s="22">
+        <v>150</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="23">
+        <v>3</v>
+      </c>
+      <c r="H12" s="24">
+        <v>42.112900000000003</v>
+      </c>
+      <c r="I12" s="1">
+        <v>27</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.93901000000000001</v>
+      </c>
+      <c r="K12" s="1">
+        <v>279.887</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.15159</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.1905</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0.22220000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="29">
+        <v>9</v>
+      </c>
+      <c r="C13" s="30">
+        <v>100</v>
+      </c>
+      <c r="D13" s="30">
+        <v>15</v>
+      </c>
+      <c r="E13" s="30">
+        <v>150</v>
+      </c>
+      <c r="F13" s="30">
+        <v>0.96</v>
+      </c>
+      <c r="G13" s="31">
+        <v>4</v>
+      </c>
+      <c r="H13" s="24">
+        <v>24.177900000000001</v>
+      </c>
+      <c r="I13" s="1">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.2331000000000001</v>
+      </c>
+      <c r="K13" s="1">
+        <v>301.42750000000001</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.19178000000000001</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.29649999999999999</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0.95830000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="29">
+        <v>10</v>
+      </c>
+      <c r="C14" s="30">
+        <v>100</v>
+      </c>
+      <c r="D14" s="30">
+        <v>20</v>
+      </c>
+      <c r="E14" s="30">
+        <v>170</v>
+      </c>
+      <c r="F14" s="30">
+        <v>0.93</v>
+      </c>
+      <c r="G14" s="31">
+        <v>3</v>
+      </c>
+      <c r="H14" s="24">
+        <v>40.386200000000002</v>
+      </c>
+      <c r="I14" s="1">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.98392999999999997</v>
+      </c>
+      <c r="K14" s="1">
+        <v>322.60000000000002</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.16434000000000001</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0.22417000000000001</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0.23330000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="29">
+        <v>11</v>
+      </c>
+      <c r="C15" s="30">
+        <v>100</v>
+      </c>
+      <c r="D15" s="30">
+        <v>25</v>
+      </c>
+      <c r="E15" s="30">
+        <v>110</v>
+      </c>
+      <c r="F15" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="G15" s="31">
+        <v>6</v>
+      </c>
+      <c r="H15" s="24">
+        <v>40.154699999999998</v>
+      </c>
+      <c r="I15" s="1">
+        <v>21</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.1865000000000001</v>
+      </c>
+      <c r="K15" s="1">
+        <v>244.58680000000001</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.13453000000000001</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.24159</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0.61899999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="29">
+        <v>12</v>
+      </c>
+      <c r="C16" s="30">
+        <v>100</v>
+      </c>
+      <c r="D16" s="30">
+        <v>30</v>
+      </c>
+      <c r="E16" s="30">
+        <v>130</v>
+      </c>
+      <c r="F16" s="30">
+        <v>0.87</v>
+      </c>
+      <c r="G16" s="31">
+        <v>5</v>
+      </c>
+      <c r="H16" s="24">
+        <v>48.195700000000002</v>
+      </c>
+      <c r="I16" s="1">
+        <v>28</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.94538</v>
+      </c>
+      <c r="K16" s="1">
+        <v>135.8048</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.15010999999999999</v>
+      </c>
+      <c r="M16" s="1">
+        <v>9.5320000000000002E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>13</v>
+      </c>
+      <c r="C17" s="30">
+        <v>120</v>
+      </c>
+      <c r="D17" s="30">
+        <v>15</v>
+      </c>
+      <c r="E17" s="30">
+        <v>170</v>
+      </c>
+      <c r="F17" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="G17" s="31">
+        <v>5</v>
+      </c>
+      <c r="H17" s="24">
+        <v>31.473299999999998</v>
+      </c>
+      <c r="I17" s="1">
+        <v>30</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.91269999999999996</v>
+      </c>
+      <c r="K17" s="1">
+        <v>238.41849999999999</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.15631</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0.13818</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>14</v>
+      </c>
+      <c r="C18" s="30">
+        <v>120</v>
+      </c>
+      <c r="D18" s="30">
+        <v>20</v>
+      </c>
+      <c r="E18" s="30">
+        <v>150</v>
+      </c>
+      <c r="F18" s="30">
+        <v>0.87</v>
+      </c>
+      <c r="G18" s="31">
+        <v>6</v>
+      </c>
+      <c r="H18" s="24">
+        <v>40.306899999999999</v>
+      </c>
+      <c r="I18" s="1">
+        <v>38</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1.0636000000000001</v>
+      </c>
+      <c r="K18" s="1">
+        <v>406.11579999999998</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.21315000000000001</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.26321</v>
+      </c>
+      <c r="N18" s="11">
+        <v>5.2600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>15</v>
+      </c>
+      <c r="C19" s="22">
+        <v>120</v>
+      </c>
+      <c r="D19" s="22">
+        <v>25</v>
+      </c>
+      <c r="E19" s="22">
+        <v>130</v>
+      </c>
+      <c r="F19" s="22">
+        <v>0.96</v>
+      </c>
+      <c r="G19" s="23">
+        <v>3</v>
+      </c>
+      <c r="H19" s="24">
+        <v>50.581099999999999</v>
+      </c>
+      <c r="I19" s="1">
+        <v>14</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1.1332</v>
+      </c>
+      <c r="K19" s="1">
+        <v>302.38670000000002</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.19635</v>
+      </c>
+      <c r="N19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4">
+        <v>16</v>
+      </c>
+      <c r="C20" s="25">
+        <v>120</v>
+      </c>
+      <c r="D20" s="26">
+        <v>30</v>
+      </c>
+      <c r="E20" s="26">
+        <v>110</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0.93</v>
+      </c>
+      <c r="G20" s="27">
+        <v>4</v>
+      </c>
+      <c r="H20" s="28">
+        <v>53.569400000000002</v>
+      </c>
+      <c r="I20" s="13">
+        <v>19</v>
+      </c>
+      <c r="J20" s="13">
+        <v>1.1503000000000001</v>
+      </c>
+      <c r="K20" s="13">
+        <v>448.7355</v>
+      </c>
+      <c r="L20" s="13">
+        <v>0.16541</v>
+      </c>
+      <c r="M20" s="13">
+        <v>0.32624999999999998</v>
+      </c>
+      <c r="N20" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFFD6F0-0A8E-4B04-A025-8C4C255898A6}">
+  <dimension ref="B3:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="C5:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="29">
+        <v>9</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="29">
+        <v>10</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="29">
+        <v>11</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="29">
+        <v>12</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>13</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>14</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>15</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4">
+        <v>16</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>